<commit_message>
export sch pdf, work on more code
code changes:
made debug header
developed mem header
changed format of headers slightly
</commit_message>
<xml_diff>
--- a/solder list.xlsx
+++ b/solder list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://okanagan365-my.sharepoint.com/personal/eddy_kneller_myokanagan_bc_ca/Documents/winter 2022/elen 227/227 project/EnviroMon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="8_{1C556247-1F5C-4CB8-BBE8-D55E9868E79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88EEDB72-60C9-4287-81EB-D33FFA59EDE1}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="8_{1C556247-1F5C-4CB8-BBE8-D55E9868E79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09D63099-E6BB-4F1A-8189-A60800AE8C56}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B8C482FE-A923-4E4C-9A08-57D4B7DFC954}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B8C482FE-A923-4E4C-9A08-57D4B7DFC954}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="173">
   <si>
     <t>BT1</t>
   </si>
@@ -509,6 +508,54 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>4.7u</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>2.2u</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>56p</t>
+  </si>
+  <si>
+    <t>1n</t>
+  </si>
+  <si>
+    <t>8p</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>3.3k</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>5.1k</t>
+  </si>
+  <si>
+    <t>4.7k</t>
   </si>
 </sst>
 </file>
@@ -758,15 +805,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{202C07A1-A555-458C-B465-96383B2ABCB5}" name="Table6" displayName="Table6" ref="A1:F51" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25">
-  <autoFilter ref="A1:F51" xr:uid="{202C07A1-A555-458C-B465-96383B2ABCB5}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{202C07A1-A555-458C-B465-96383B2ABCB5}" name="Table6" displayName="Table6" ref="A1:G51" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25">
+  <autoFilter ref="A1:G51" xr:uid="{202C07A1-A555-458C-B465-96383B2ABCB5}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{0285181E-67FF-4F62-ACEC-49B6CB0EF29F}" name="Designator" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{21B323D1-57FF-4440-B4CC-BEFE411E2500}" name="Quantity"/>
     <tableColumn id="3" xr3:uid="{D4817779-B440-4AA0-834A-EBF1B9EBB450}" name="Description" dataDxfId="23"/>
     <tableColumn id="4" xr3:uid="{1EC644D3-1148-4805-BDB2-A34972046DFC}" name="Name" dataDxfId="22"/>
     <tableColumn id="5" xr3:uid="{0CC05657-FD2F-4566-957B-49CBA09F3429}" name="Manufacturer" dataDxfId="21"/>
     <tableColumn id="6" xr3:uid="{F84668E1-AC65-48C9-A060-0F2DDD7FE107}" name="Part Number"/>
+    <tableColumn id="7" xr3:uid="{5B5363A0-14F3-4E74-8391-F7D8574E337C}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1114,932 +1162,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{778A81FC-01FC-4D71-A4AB-18EA4B5B46D5}">
-  <dimension ref="A1:F51"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>782763102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15">
-        <v>10</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <v>782763102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F26"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27">
-        <v>5</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29">
-        <v>5</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F29"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F32"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F33" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F35"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F38"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F39"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B41">
-        <v>3</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F41"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F42" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F43" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F44" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F45" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F46" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F47" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F48" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F49" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F50"/>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F51" t="s">
-        <v>150</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1795B871-BB89-4F95-9970-A4BE16F3CC34}">
-  <dimension ref="A1:G40"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,6 +1185,986 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>782763102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27"/>
+      <c r="G27" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28"/>
+      <c r="G28" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29"/>
+      <c r="G29" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30" s="1">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32"/>
+      <c r="G32" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34"/>
+      <c r="G34" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35"/>
+      <c r="G35" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36"/>
+      <c r="G36" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37"/>
+      <c r="G37" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F48" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="66" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1795B871-BB89-4F95-9970-A4BE16F3CC34}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="2.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>151</v>
       </c>
@@ -2787,7 +2896,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -2796,10 +2905,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F993CB2-CE4F-4680-94E0-C7EA7EBCD35E}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3027,7 +3139,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -3036,10 +3148,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3FB8CC-252B-47FB-8079-5A2A27A45A4A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3234,7 +3349,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>